<commit_message>
proj 6 - part 1
</commit_message>
<xml_diff>
--- a/OptimalizationLabs1/proj5_Izworski_Jarek_Klimczyk.xlsx
+++ b/OptimalizationLabs1/proj5_Izworski_Jarek_Klimczyk.xlsx
@@ -3,31 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C637FAB-5A41-4D9E-A485-D4BC9861E2EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BFAFC-AA54-4DA3-862A-1889F34FD46B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabela 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Tabela 1'!$P$3:$P$103</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Tabela 1'!$Q$3:$Q$103</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Tabela 2'!$F$2:$F$102</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Tabela 2'!$G$2:$G$102</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Tabela 2'!$F$2:$F$102</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Tabela 2'!$G$2:$G$102</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Tabela 2'!$F$2:$F$102</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Tabela 2'!$G$2:$G$102</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Tabela 1'!$K$3:$K$103</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Tabela 1'!$L$3:$L$103</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Tabela 1'!$K$3:$K$103</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Tabela 1'!$L$3:$L$103</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Tabela 1'!$P$3:$P$103</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Tabela 1'!$Q$3:$Q$103</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Tabela 1'!$F$3:$F$103</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Tabela 1'!$G$3:$G$103</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Tabela 1'!$P$3:$P$103</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Tabela 1'!$Q$3:$Q$103</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Tabela 2'!$F$2:$F$102</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Tabela 2'!$G$2:$G$102</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Tabela 2'!$F$2:$F$102</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Tabela 2'!$G$2:$G$102</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -957,12 +949,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1087,12 +1079,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1217,12 +1209,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3583,7 +3575,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2893518" y="20417438"/>
+              <a:off x="2893518" y="20416077"/>
               <a:ext cx="4549588" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3661,7 +3653,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8030614" y="20519892"/>
+              <a:off x="8030614" y="20518531"/>
               <a:ext cx="4549589" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3739,7 +3731,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13219739" y="20495880"/>
+              <a:off x="13219739" y="20494519"/>
               <a:ext cx="4549588" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3822,8 +3814,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8472769" y="698966"/>
-              <a:ext cx="4594412" cy="2743200"/>
+              <a:off x="8438031" y="698966"/>
+              <a:ext cx="4625788" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4179,7 +4171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
@@ -9946,8 +9938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>